<commit_message>
Fix formating Issue in KB files
</commit_message>
<xml_diff>
--- a/KB/CTLS-Guide-fr.xlsx
+++ b/KB/CTLS-Guide-fr.xlsx
@@ -39,17 +39,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Qu'est-ce que le Système de suivi du cannabis et de demandes de licences (SSCDL) ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Le nom de l'application Web et du système de gestion de cas établis et entretenus par Santé Canada par l'intermédiaire duquel les demandeurs peuvent présenter une demande de licence de cannabis qui sera délivrée par Santé Canada, et par l'entremise de laquelle les exigences de suivi mensuelles doivent être soumises. </t>
+      <t xml:space="preserve">Qu'est-ce que le Système de suivi du cannabis et de demandes de licences (SSCDL) ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Le nom de l'application Web et du système de gestion de cas établis et entretenus par Santé Canada par l'intermédiaire duquel les demandeurs peuvent présenter une demande de licence de cannabis qui sera délivrée par Santé Canada, et par l'entremise de laquelle les exigences de suivi mensuelles doivent être soumises. </t>
     </r>
   </si>
   <si>
@@ -64,17 +64,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Qu'est-ce que l'Accès de niveau redditionnel ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Désigne le niveau d'accès des personnes inscrites au SSCDL qui sont autorisées à présenter des rapports mensuels. Présentement, l'accès de niveau redditionnel est accordé uniquement à la personne désignée comme responsable. </t>
+      <t xml:space="preserve">Qu'est-ce que l'Accès de niveau redditionnel ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Désigne le niveau d'accès des personnes inscrites au SSCDL qui sont autorisées à présenter des rapports mensuels. Présentement, l'accès de niveau redditionnel est accordé uniquement à la personne désignée comme responsable. </t>
     </r>
   </si>
   <si>
@@ -89,17 +89,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Qu'est-ce qu'un Lieu ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">À l'égard d'un titulaire de licence, emplacement à l'usage exclusif de ce dernier et comprenant au moins un bâtiment ou une partie de bâtiment. </t>
+      <t xml:space="preserve">Qu'est-ce qu'un Lieu ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+À l'égard d'un titulaire de licence, emplacement à l'usage exclusif de ce dernier et comprenant au moins un bâtiment ou une partie de bâtiment. </t>
     </r>
   </si>
   <si>
@@ -114,17 +114,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Qu'est-ce qu'un Produit du cannabis ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Cannabis d'une seule des catégories visées à l'annexe 4 de la Loi ou tout accessoire qui contient de ce cannabis, une fois emballé et étiqueté pour la vente au détail aux consommateurs. Sont exclues de la présente définition, les drogues contenant du cannabis. </t>
+      <t xml:space="preserve">Qu'est-ce qu'un Produit du cannabis ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Cannabis d'une seule des catégories visées à l'annexe 4 de la Loi ou tout accessoire qui contient de ce cannabis, une fois emballé et étiqueté pour la vente au détail aux consommateurs. Sont exclues de la présente définition, les drogues contenant du cannabis. </t>
     </r>
   </si>
   <si>
@@ -139,17 +139,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Qu'est-ce qu'un Inventaire final ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Fait référence à la quantité de produits de cannabis finis. Les quantités ne concernent que le cannabis et ne doivent pas inclure d'emballage ou d'accessoires. Les catégories de cannabis qui sont peut-être des produits de cannabis sont celles qui figurent à l'annexe 4 de la Loi sur le cannabis. (graines, plantes, cannabis séché, cannabis frais, huile de cannabis).</t>
+      <t xml:space="preserve">Qu'est-ce qu'un Inventaire final ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Fait référence à la quantité de produits de cannabis finis. Les quantités ne concernent que le cannabis et ne doivent pas inclure d'emballage ou d'accessoires. Les catégories de cannabis qui sont peut-être des produits de cannabis sont celles qui figurent à l'annexe 4 de la Loi sur le cannabis. (graines, plantes, cannabis séché, cannabis frais, huile de cannabis).</t>
     </r>
   </si>
   <si>
@@ -164,17 +164,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Qu'est-ce qu'un Inventaire des produits non finis ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Signifie la quantité de cannabis qui n'est pas une autre substance que le cannabis contenu dans un produit de cannabis. Les catégories de cannabis reflètent celles de l'inventaire de cannabis fini, en plus des «autres» catégories de cannabis ne figurant pas dans la liste de l'annexe 4 de la Loi sur le cannabis (p. ex., produits comestibles ou concentrés mis au point à des fins de recherche et qui ne sont pas destinés à la vente). </t>
+      <t xml:space="preserve">Qu'est-ce qu'un Inventaire des produits non finis ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Signifie la quantité de cannabis qui n'est pas une autre substance que le cannabis contenu dans un produit de cannabis. Les catégories de cannabis reflètent celles de l'inventaire de cannabis fini, en plus des «autres» catégories de cannabis ne figurant pas dans la liste de l'annexe 4 de la Loi sur le cannabis (p. ex., produits comestibles ou concentrés mis au point à des fins de recherche et qui ne sont pas destinés à la vente). </t>
     </r>
   </si>
   <si>
@@ -189,17 +189,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Qu'est-ce qu'un Inventaire à la date d'ouverture ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Désigne le montant figurant à l'inventaire le premier jour de la période de rapport. </t>
+      <t xml:space="preserve">Qu'est-ce qu'un Inventaire à la date d'ouverture ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Désigne le montant figurant à l'inventaire le premier jour de la période de rapport. </t>
     </r>
   </si>
   <si>
@@ -214,17 +214,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Qu'est-ce que la Production ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Fait référence aux ajouts de cannabis par le biais d'activités menées sur le site. </t>
+      <t xml:space="preserve">Qu'est-ce que la Production ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Fait référence aux ajouts de cannabis par le biais d'activités menées sur le site. </t>
     </r>
   </si>
   <si>
@@ -239,17 +239,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Que signifie Transformé ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Signifie que le cannabis est produit d'une classe de cannabis à une autre (par exemple, du cannabis séché à l'huile de cannabis). Enregistré comme une réduction à l'inventaire de la classe de cannabis à partir de laquelle la nouvelle classe de cannabis a été produite. </t>
+      <t xml:space="preserve">Que signifie Transformé ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Signifie que le cannabis est produit d'une classe de cannabis à une autre (par exemple, du cannabis séché à l'huile de cannabis). Enregistré comme une réduction à l'inventaire de la classe de cannabis à partir de laquelle la nouvelle classe de cannabis a été produite. </t>
     </r>
   </si>
   <si>
@@ -264,17 +264,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Que signifie emballé et étiqueté ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Signifie emballés et étiquetés comme un produit de cannabis. Cela devrait être enregistré à la fois comme une réduction à l'inventaire des produits non finis et un ajout à l'inventaire final. </t>
+      <t xml:space="preserve">Que signifie emballé et étiqueté ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Signifie emballés et étiquetés comme un produit de cannabis. Cela devrait être enregistré à la fois comme une réduction à l'inventaire des produits non finis et un ajout à l'inventaire final. </t>
     </r>
   </si>
   <si>
@@ -289,17 +289,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Que sont les Importations / Exportations ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Signifie le mouvement du cannabis au Canada et à l'étranger. En ce qui concerne les rapports, ils doivent être inclus dans le cannabis qui n'est pas un produit du cannabis et être inscrits dans l'inventaire des produits non finis. </t>
+      <t xml:space="preserve">Que sont les Importations / Exportations ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Signifie le mouvement du cannabis au Canada et à l'étranger. En ce qui concerne les rapports, ils doivent être inclus dans le cannabis qui n'est pas un produit du cannabis et être inscrits dans l'inventaire des produits non finis. </t>
     </r>
   </si>
   <si>
@@ -314,17 +314,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Que sont les Retours ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Il s'agit du cannabis précédemment vendu / acheté et distribué à un autre titulaire de licence ou à un consommateur au niveau de la vente au détail et retourné par la suite. Le cannabis envoyé hors site pour être testé ou traité et retourné par la suite au même titulaire de licence devrait être enregistré en tant que distribution vers / à partir de la catégorie de licence applicable. </t>
+      <t xml:space="preserve">Que sont les Retours ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Il s'agit du cannabis précédemment vendu / acheté et distribué à un autre titulaire de licence ou à un consommateur au niveau de la vente au détail et retourné par la suite. Le cannabis envoyé hors site pour être testé ou traité et retourné par la suite au même titulaire de licence devrait être enregistré en tant que distribution vers / à partir de la catégorie de licence applicable. </t>
     </r>
   </si>
   <si>
@@ -339,17 +339,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Que signifie Détruit ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Signifie du cannabis qui a été détruit sur place ou envoyé pour être détruit hors site. </t>
+      <t xml:space="preserve">Que signifie Détruit ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Signifie du cannabis qui a été détruit sur place ou envoyé pour être détruit hors site. </t>
     </r>
   </si>
   <si>
@@ -364,17 +364,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Que sont les Pertes liées au séchage et à la transformation ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Signifie que la masse de cannabis est réduite en raison de la perte au séchage ou d'autres activités de traitement. </t>
+      <t xml:space="preserve">Que sont les Pertes liées au séchage et à la transformation ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Signifie que la masse de cannabis est réduite en raison de la perte au séchage ou d'autres activités de traitement. </t>
     </r>
   </si>
   <si>
@@ -389,17 +389,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Que signifie Autre ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Dans le contexte du mouvement du cannabis, il s'agit d'ajouts ou de réductions d'inventaire qui ne sont applicables à aucune autre catégorie. Dans le contexte du cannabis, cela signifie que les catégories de cannabis ne figurent pas dans l'annexe 4 de la Loi sur le cannabis par exemple, les produits comestibles ou concentrés développés à des fins de recherche et nondestinés à la vente). </t>
+      <t xml:space="preserve">Que signifie Autre ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Dans le contexte du mouvement du cannabis, il s'agit d'ajouts ou de réductions d'inventaire qui ne sont applicables à aucune autre catégorie. Dans le contexte du cannabis, cela signifie que les catégories de cannabis ne figurent pas dans l'annexe 4 de la Loi sur le cannabis par exemple, les produits comestibles ou concentrés développés à des fins de recherche et nondestinés à la vente). </t>
     </r>
   </si>
   <si>
@@ -414,17 +414,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Que sont les Ventes - Médical ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Signifie vente aux clients enregistrés à des fins médicales. Les titulaires d'une licence de culture ou d'une licence de transformation qui expédient du cannabis directement à un client enregistré pour le compte d'un titulaire d'une licence de vente à des fins médicales doivent consigner cela comme une vente de cannabis à des fins médicales. </t>
+      <t xml:space="preserve">Que sont les Ventes - Médical ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Signifie vente aux clients enregistrés à des fins médicales. Les titulaires d'une licence de culture ou d'une licence de transformation qui expédient du cannabis directement à un client enregistré pour le compte d'un titulaire d'une licence de vente à des fins médicales doivent consigner cela comme une vente de cannabis à des fins médicales. </t>
     </r>
   </si>
   <si>
@@ -439,17 +439,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Que sont les Ventes - non médical pour le distributeur / détaillant ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Désigne la vente de produits de cannabis à un vendeur sous autorisation provinciale. Cela peut aller d'un transformateur sous licence fédérale à un distributeur / détaillant, ou d'un distributeur / détaillant à un autre distributeur / détaillant. </t>
+      <t xml:space="preserve">Que sont les Ventes - non médical pour le distributeur / détaillant ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Désigne la vente de produits de cannabis à un vendeur sous autorisation provinciale. Cela peut aller d'un transformateur sous licence fédérale à un distributeur / détaillant, ou d'un distributeur / détaillant à un autre distributeur / détaillant. </t>
     </r>
   </si>
   <si>
@@ -464,17 +464,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Que sont les Ventes - non médical en ligne ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Désigne les ventes aux consommateurs au niveau de la vente au détail qui n'étaient pas présentes sur le site au moment de l'achat. Cela comprend les ventes effectuées en ligne ou par téléphone. Les titulaires de licences fédérales qui expédient du cannabis au nom d'une autorité provinciale ou territoriale directement à un consommateur au niveau de la vente au détail qui a passé une commande par l'intermédiaire d'un système en ligne provincial ou territorial devraient le consigner en tant que vente en ligne à des fins non médicales directe aux consommateurs. </t>
+      <t xml:space="preserve">Que sont les Ventes - non médical en ligne ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Désigne les ventes aux consommateurs au niveau de la vente au détail qui n'étaient pas présentes sur le site au moment de l'achat. Cela comprend les ventes effectuées en ligne ou par téléphone. Les titulaires de licences fédérales qui expédient du cannabis au nom d'une autorité provinciale ou territoriale directement à un consommateur au niveau de la vente au détail qui a passé une commande par l'intermédiaire d'un système en ligne provincial ou territorial devraient le consigner en tant que vente en ligne à des fins non médicales directe aux consommateurs. </t>
     </r>
   </si>
   <si>
@@ -489,17 +489,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Que sont les Employés ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Ce sont des personnes qui, au cours de la période de référence, travaillaient à l'établissement chargé des rapports, quel que soit le nombre d'heures travaillées. Cela inclut les entrepreneurs et les agents.
+      <t xml:space="preserve">Que sont les Employés ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Ce sont des personnes qui, au cours de la période de référence, travaillaient à l'établissement chargé des rapports, quel que soit le nombre d'heures travaillées. Cela inclut les entrepreneurs et les agents.
 * </t>
     </r>
     <r>
@@ -510,16 +510,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Gestion </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">: Comprend les cadres supérieurs et intermédiaires de gestion des employés.
+      <t xml:space="preserve">Gestion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> : Comprend les cadres supérieurs et intermédiaires de gestion des employés.
 * </t>
     </r>
     <r>
@@ -550,16 +550,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Ventes </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">: Comprend les employés de la vente de détail et de gros, du service à la clientèle.
+      <t xml:space="preserve">Ventes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> : Comprend les employés de la vente de détail et de gros, du service à la clientèle.
 * </t>
     </r>
     <r>
@@ -590,16 +590,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Autres </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">: Comprend tous les autres employés. </t>
+      <t xml:space="preserve">Autres</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> : Comprend tous les autres employés. </t>
     </r>
   </si>
   <si>
@@ -614,17 +614,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Qu'est-ce que la Capacité?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Renvoie à la zone où les plantes de cannabis sont cultivées, reproduites récoltées, ou séchées.
+      <t xml:space="preserve">Qu'est-ce que la Capacité?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Renvoie à la zone où les plantes de cannabis sont cultivées, reproduites récoltées, ou séchées.
 * </t>
     </r>
     <r>
@@ -635,16 +635,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Zone de floraison </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">: zone où toutes les plantes de cannabis sont cultivées en vue de la récolte.
+      <t xml:space="preserve">Zone de floraison</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> : zone où toutes les plantes de cannabis sont cultivées en vue de la récolte.
 * </t>
     </r>
     <r>
@@ -675,16 +675,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Salle de clonage </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">: Salle qui contient des semis/des clones.
+      <t xml:space="preserve">Salle de clonage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> : Salle qui contient des semis/des clones.
 * </t>
     </r>
     <r>
@@ -695,16 +695,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Salle de séchage </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">: zone où le cannabis récolté est soumis à un processus de séchage. </t>
+      <t xml:space="preserve">Salle de séchage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> : zone où le cannabis récolté est soumis à un processus de séchage. </t>
     </r>
   </si>
   <si>
@@ -719,17 +719,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Qu'est-ce que l'Accès à des fins médicales ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Renvoie aux éléments de données portant sur la fourniture du cannabis à des fins médicales qui doivent être soumis par les titulaires de licences pour la vente. </t>
+      <t xml:space="preserve">Qu'est-ce que l'Accès à des fins médicales ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Renvoie aux éléments de données portant sur la fourniture du cannabis à des fins médicales qui doivent être soumis par les titulaires de licences pour la vente. </t>
     </r>
   </si>
   <si>
@@ -744,17 +744,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Que sont les Montants autorisés ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Fait référence à la quantité de cannabis à des fins médicales, mesurée en grammes de cannabis séché par jour, autorisée par un professionnel de la santé (PS).
+      <t xml:space="preserve">Que sont les Montants autorisés ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Fait référence à la quantité de cannabis à des fins médicales, mesurée en grammes de cannabis séché par jour, autorisée par un professionnel de la santé (PS).
 Les symboles suivants seront utilisés tout au long du présent guide afin de souligner des renseignements précis. </t>
     </r>
   </si>
@@ -795,17 +795,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Pourquoi seule la personne désignée comme responsable peut avoir un accès de niveau redditionnel pour soumettre des rapports mensuels?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Afin de réduire au minimum les risques et d'assurer la qualité des données, seule la personne désignée comme titulaire de licence (ou dans le cas d'une société, l'autorité administrative) ou la personne désignée comme responsable se voit accorder un accès au niveau de rapport et est autorisée à soumettre des rapports conformément à la Politique sur la sécurité du gouvernement et à sa Norme sur l'assurance de l'identité et des justificatifs. Toutefois, d'autres membres de votre organisation peuvent préparer le document. csv pour que cette personne puisse procéder au téléchargement.
+      <t xml:space="preserve">Pourquoi seule la personne désignée comme responsable peut avoir un accès de niveau redditionnel pour soumettre des rapports mensuels?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Afin de réduire au minimum les risques et d'assurer la qualité des données, seule la personne désignée comme titulaire de licence (ou dans le cas d'une société, l'autorité administrative) ou la personne désignée comme responsable se voit accorder un accès au niveau de rapport et est autorisée à soumettre des rapports conformément à la Politique sur la sécurité du gouvernement et à sa Norme sur l'assurance de l'identité et des justificatifs. Toutefois, d'autres membres de votre organisation peuvent préparer le document. csv pour que cette personne puisse procéder au téléchargement.
 Veuillez noter, dans le cadre de la prochaine version du système, il est envisagé d'accorder cette fonction à d'autre personnel ayant l'habilitaton de sécurité nécessaire. </t>
     </r>
   </si>
@@ -821,17 +821,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Comment enregistrer les marchandises en transit ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Au moment de l'établissement des rapports, les marchandises en transit doivent être recensées selon les modalités d'expédition des marchandises, à savoir :
+      <t xml:space="preserve">Comment enregistrer les marchandises en transit ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Au moment de l'établissement des rapports, les marchandises en transit doivent être recensées selon les modalités d'expédition des marchandises, à savoir :
 Point d'expédition FAB : Si l'expédition est désignée comme point d'expédition fret à bord (FAB), le droit de propriété est transféré à l'acheteur dès que le vendeur expédie la commande.
 Destination FAB : Si l'expédition est désignée comme destination fret à bord (FAB), le droit de propriété est transféré à l'acheteur dès que celui-ci reçoit la commande. </t>
     </r>
@@ -848,17 +848,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Comment le "cannabis frais" doit-il être comptabilisé dans l'inventaire des produits non finis ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Dans la version précédente de ce document d'orientation, il était indiqué qu'aux fins du SSC, le cannabis frais ne doit être enregistré dans l'inventaire des produits non finis que s'il est destiné à être vendu sous cette forme. Après mûre réflexion, nous demandons maintenant que cette catégorie soit utilisée pour indiquer le poids du cannabis mouillé récolté et toute perte due au séchage ou à la transformation avant de catégoriser le stock comme suit : «Non fini - Cannabis séché».
+      <t xml:space="preserve">Comment le "cannabis frais" doit-il être comptabilisé dans l'inventaire des produits non finis ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Dans la version précédente de ce document d'orientation, il était indiqué qu'aux fins du SSC, le cannabis frais ne doit être enregistré dans l'inventaire des produits non finis que s'il est destiné à être vendu sous cette forme. Après mûre réflexion, nous demandons maintenant que cette catégorie soit utilisée pour indiquer le poids du cannabis mouillé récolté et toute perte due au séchage ou à la transformation avant de catégoriser le stock comme suit : «Non fini – Cannabis séché».
 En d'autres mots, le poids mouillé récolté initial devrait être enregistré comme suit : «Non fini - Cannabis frais - Ajout - quantité produite».
 La perte du poids due au séchage devrait être enregistrée comme suit : «Non fini - Cannabis frais - Réductions - Perte séchage/transformation».
 La quantité restante qui doit être transformée davantage en tant que cannabis séché devrait être enregistrée comme suit : «Non fini - Cannabis frais - Réductions - quantité transformée» ainsi que «Non fini - Cannabis séché - Additions - quantité produite».
@@ -877,17 +877,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Comment dois-je comptabiliser les produits en cours de séchage à la fin du mois ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">En ce qui concerne la perte de séchage / transformation du cannabis frais, les estimations sont acceptables pour le produit en cours de séchage en fin de mois. Les méthodes d'estimation devraient être disponibles sur demande de Santé Canada. </t>
+      <t xml:space="preserve">Comment dois-je comptabiliser les produits en cours de séchage à la fin du mois ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+En ce qui concerne la perte de séchage / transformation du cannabis frais, les estimations sont acceptables pour le produit en cours de séchage en fin de mois. Les méthodes d'estimation devraient être disponibles sur demande de Santé Canada. </t>
     </r>
   </si>
   <si>
@@ -902,17 +902,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Comment dois-je comptabiliser les déchets végétaux ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Il a été noté que puisque les plantes de cannabis sont mesurées en unités individuelles, les déclarants ne sont pas en mesure d'enregistrer la destruction partielle des matières végétales, comme les taillages vivants. Jusqu'à la prochaine version du Système de suivi du cannabis et de demande de licence, ces déchets végétaux devraient d'abord être enregistrés comme suit : «Non fini - Autre - Ajout - Production». Une fois détruits, ils devaient être enregistrés comme suit : «Non fini - Autre - Réduction - Détruit» mesuré en kilogrammes. </t>
+      <t xml:space="preserve">Comment dois-je comptabiliser les déchets végétaux ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Il a été noté que puisque les plantes de cannabis sont mesurées en unités individuelles, les déclarants ne sont pas en mesure d'enregistrer la destruction partielle des matières végétales, comme les taillages vivants. Jusqu'à la prochaine version du Système de suivi du cannabis et de demande de licence, ces déchets végétaux devraient d'abord être enregistrés comme suit : «Non fini - Autre - Ajout - Production». Une fois détruits, ils devaient être enregistrés comme suit : «Non fini - Autre - Réduction - Détruit» mesuré en kilogrammes. </t>
     </r>
   </si>
   <si>
@@ -927,17 +927,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Comment devrais-je comptabiliser les ajouts ultérieurs d'huiles de base à de l'huile de cannabis non fini ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Cela devrait être saisi comme un ajout à l'huile de cannabis non fini - Production. </t>
+      <t xml:space="preserve">Comment devrais-je comptabiliser les ajouts ultérieurs d'huiles de base à de l'huile de cannabis non fini ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Cela devrait être saisi comme un ajout à l'huile de cannabis non fini - Production. </t>
     </r>
   </si>
   <si>
@@ -952,17 +952,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Comment dois-je rapporter les capsules d'huile ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Les capsules d'huile doivent être enregistrées comme de l'huile de cannabis. Le volume doit être enregistré net de tout matériau d'encapsulation conformêment aux exigences en matière d'étiquetage du Règlement sur le cannabis. </t>
+      <t xml:space="preserve">Comment dois-je rapporter les capsules d'huile ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Les capsules d'huile doivent être enregistrées comme de l'huile de cannabis. Le volume doit être enregistré net de tout matériau d'encapsulation conformêment aux exigences en matière d'étiquetage du Règlement sur le cannabis. </t>
     </r>
   </si>
   <si>
@@ -977,17 +977,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Comment devrais-je comptabiliser le poids des matériaux détruits autres que le cannabis qui contiennent des résidus ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Le poids du matériel détruit non-cannabis qui contient des résidus (serviettes, ruban d'encapsulation, etc.) n'a pas besoin d'être inclus dans le rapport du SSC, ni la méthode de destruction du cannabis ne doit pas être inclus dans le rapport du SSC. Toutefois, notez que, conformêment au paragraphe 229 (1) du règlement, vous devez conserver un document contenant les détails de la destruction du cannabis:
+      <t xml:space="preserve">Comment devrais-je comptabiliser le poids des matériaux détruits autres que le cannabis qui contiennent des résidus ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Le poids du matériel détruit non-cannabis qui contient des résidus (serviettes, ruban d'encapsulation, etc.) n'a pas besoin d'être inclus dans le rapport du SSC, ni la méthode de destruction du cannabis ne doit pas être inclus dans le rapport du SSC. Toutefois, notez que, conformêment au paragraphe 229 (1) du règlement, vous devez conserver un document contenant les détails de la destruction du cannabis:
 229 (1) Le titulaire d'une licence - autre qu'une licence relative aux drogues contenant du cannabis - conserve un document qui contient les renseignements ci-après chaque fois qu'il détruit ou fait détruire du cannabis :
 1. la description et, le cas échéant, le nom commercial du cannabis;
 2. la date à laquelle il est détruit et, à cette date, son poids net - ou, s'il s'agit d'huile de cannabis, son poids ou volume net - avant la destruction;
@@ -1008,17 +1008,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Dois-je enregistrer les expéditions directes aux clients qui ont passé leur commande à partir d'un système provincial / territorial de vente en ligne de cannabis ?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Les commandes en ligne enregistrées par un distributeur ou un détaillant, mais envoyées directement à un consommateur au détail par le titulaire de licence fédérale doivent être enregistrées comme une vente en ligne non médicale par le titulaire de licence fédérale. Le distributeur ou le détaillant ne doit pas enregistrer la vente. </t>
+      <t xml:space="preserve">Dois-je enregistrer les expéditions directes aux clients qui ont passé leur commande à partir d'un système provincial / territorial de vente en ligne de cannabis ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Les commandes en ligne enregistrées par un distributeur ou un détaillant, mais envoyées directement à un consommateur au détail par le titulaire de licence fédérale doivent être enregistrées comme une vente en ligne non médicale par le titulaire de licence fédérale. Le distributeur ou le détaillant ne doit pas enregistrer la vente. </t>
     </r>
   </si>
   <si>
@@ -1033,17 +1033,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Aide et assistance dans le cadre du SSCDL 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Si vous avez des questions au sujet de la soumission de rapports mensuels via le SSCDL, vous pouvez demander de l'assistance en nous envoyant un courriel à l'adresse hc.ctls-bi-sscdl-ie.sc@canada.ca. Veillez à inscrire Rapports SSCDL dans la ligne objet du courriel, pour vous assurer que votre demande est adressée à l'expert en la matière appropriée. Si votre demande concerne une erreur reçue pendant le processus de soumission, fournissez autant de détails que possible, y compris des captures d'écran et dans le cas d'un téléchargement de fichier, une copie du fichier .csv que vous avez tenté de soumettre. </t>
+      <t xml:space="preserve">Aide et assistance dans le cadre du SSCDL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Si vous avez des questions au sujet de la soumission de rapports mensuels via le SSCDL, vous pouvez demander de l'assistance en nous envoyant un courriel à l'adresse hc.ctls-bi-sscdl-ie.sc@canada.ca. Veillez à inscrire Rapports SSCDL dans la ligne objet du courriel, pour vous assurer que votre demande est adressée à l'expert en la matière appropriée. Si votre demande concerne une erreur reçue pendant le processus de soumission, fournissez autant de détails que possible, y compris des captures d'écran et dans le cas d'un téléchargement de fichier, une copie du fichier .csv que vous avez tenté de soumettre. </t>
     </r>
   </si>
   <si>
@@ -1058,17 +1058,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Comment importer du cannabis?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Vous ne pouvez pas importer de cannabis au Canada.</t>
+      <t xml:space="preserve">Comment importer du cannabis?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Vous ne pouvez pas importer de cannabis au Canada.</t>
     </r>
   </si>
   <si>
@@ -1083,17 +1083,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Comment exporter du cannabis?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Vous ne pouvez pas exporter de cannabis du Canada.</t>
+      <t xml:space="preserve">Comment exporter du cannabis?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Vous ne pouvez pas exporter de cannabis du Canada.</t>
     </r>
   </si>
 </sst>
@@ -1218,8 +1218,8 @@
   </sheetPr>
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>